<commit_message>
consistent version for pf.t1
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_SJPF_Decrements_AV2019.xlsx
+++ b/inputs/data_raw/Data_SJPF_Decrements_AV2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_SJ\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B821AE-BA9D-4127-8364-B5425C9980DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C257B26A-0458-40EF-A43A-C5E955324648}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="43" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="70">
   <si>
     <t>TOC</t>
   </si>
@@ -345,9 +345,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>yos_15.19</t>
-  </si>
-  <si>
     <t>yos_20.24</t>
   </si>
   <si>
@@ -366,9 +363,6 @@
     <t>C7:D19</t>
   </si>
   <si>
-    <t>C6:H33</t>
-  </si>
-  <si>
     <t>C6:F32</t>
   </si>
   <si>
@@ -376,6 +370,12 @@
   </si>
   <si>
     <t>C6:E46</t>
+  </si>
+  <si>
+    <t>yos_5.19</t>
+  </si>
+  <si>
+    <t>C6:H38</t>
   </si>
 </sst>
 </file>
@@ -1026,13 +1026,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>524472</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>19368</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1270,15 +1270,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>467359</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>304</xdr:rowOff>
+      <xdr:colOff>162559</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171754</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1301,7 +1301,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6648450" y="2895600"/>
+          <a:off x="6343650" y="2495550"/>
           <a:ext cx="4544059" cy="2181529"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1314,15 +1314,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>581622</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>66993</xdr:rowOff>
+      <xdr:colOff>181572</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1345,7 +1345,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7029450" y="5343525"/>
+          <a:off x="6629400" y="4733925"/>
           <a:ext cx="4277322" cy="2276793"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1697,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F0179D-30E8-4C62-9A5E-014F54719930}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G35"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,16 +1762,16 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
         <v>59</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>60</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>61</v>
-      </c>
-      <c r="G8" t="s">
-        <v>62</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="30"/>
@@ -2740,7 +2740,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -3672,8 +3672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3816633E-6322-417C-AE1E-F43C2AF11311}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3693,7 +3693,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3720,7 +3720,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3882,7 +3882,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3900,7 +3900,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3921,7 +3921,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -4308,10 +4308,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BB2C82-1C12-483D-B657-F4147BFD0186}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4329,7 +4329,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4350,31 +4350,30 @@
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>60</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>61</v>
       </c>
-      <c r="H6" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
       <c r="C7" t="s">
         <v>50</v>
       </c>
       <c r="D7">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>0.02</v>
@@ -4390,12 +4389,11 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
       <c r="C8" t="s">
         <v>50</v>
       </c>
       <c r="D8">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>0.02</v>
@@ -4411,66 +4409,63 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
       <c r="C9" t="s">
         <v>50</v>
       </c>
       <c r="D9">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E9">
-        <v>7.4999999999999997E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G9">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
       <c r="C10" t="s">
         <v>50</v>
       </c>
       <c r="D10">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E10">
-        <v>7.4999999999999997E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F10">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G10">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
       <c r="C11" t="s">
         <v>50</v>
       </c>
       <c r="D11">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F11">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G11">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4479,19 +4474,19 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E12">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="F12">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="G12">
-        <v>0.35</v>
+        <v>0.02</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4500,19 +4495,19 @@
         <v>50</v>
       </c>
       <c r="D13">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E13">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="F13">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="G13">
-        <v>0.35</v>
+        <v>0.02</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4521,16 +4516,16 @@
         <v>50</v>
       </c>
       <c r="D14">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E14">
-        <v>0.25</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G14">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -4542,16 +4537,16 @@
         <v>50</v>
       </c>
       <c r="D15">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E15">
-        <v>0.25</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G15">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -4563,16 +4558,16 @@
         <v>50</v>
       </c>
       <c r="D16">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E16">
-        <v>0.25</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F16">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G16">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -4584,16 +4579,16 @@
         <v>50</v>
       </c>
       <c r="D17">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -4602,111 +4597,115 @@
     <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E18">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F18">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="G18">
-        <v>0.01</v>
+        <v>0.35</v>
       </c>
       <c r="H18">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E19">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
       <c r="F19">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="G19">
-        <v>0.01</v>
+        <v>0.75</v>
       </c>
       <c r="H19">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="11"/>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E20">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
       <c r="F20">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="G20">
-        <v>0.01</v>
+        <v>0.75</v>
       </c>
       <c r="H20">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="11"/>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E21">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
       <c r="F21">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
-        <v>0.01</v>
+        <v>0.75</v>
       </c>
       <c r="H21">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E22">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
       <c r="C23" t="s">
         <v>51</v>
       </c>
       <c r="D23">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E23">
         <v>0.01</v>
@@ -4721,12 +4720,13 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="17"/>
       <c r="C24" t="s">
         <v>51</v>
       </c>
       <c r="D24">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E24">
         <v>0.01</v>
@@ -4746,19 +4746,19 @@
         <v>51</v>
       </c>
       <c r="D25">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E25">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F25">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G25">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -4766,19 +4766,19 @@
         <v>51</v>
       </c>
       <c r="D26">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E26">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F26">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G26">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -4786,19 +4786,19 @@
         <v>51</v>
       </c>
       <c r="D27">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E27">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F27">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G27">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -4806,19 +4806,19 @@
         <v>51</v>
       </c>
       <c r="D28">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E28">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F28">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="G28">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -4826,19 +4826,19 @@
         <v>51</v>
       </c>
       <c r="D29">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E29">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F29">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="G29">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -4846,16 +4846,16 @@
         <v>51</v>
       </c>
       <c r="D30">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E30">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F30">
-        <v>0.35</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G30">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -4866,16 +4866,16 @@
         <v>51</v>
       </c>
       <c r="D31">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E31">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F31">
-        <v>0.35</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G31">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -4886,16 +4886,16 @@
         <v>51</v>
       </c>
       <c r="D32">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E32">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F32">
-        <v>0.35</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G32">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -4906,18 +4906,118 @@
         <v>51</v>
       </c>
       <c r="D33">
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.15</v>
+      </c>
+      <c r="G33">
+        <v>0.25</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34">
+        <v>61</v>
+      </c>
+      <c r="E34">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F34">
+        <v>0.15</v>
+      </c>
+      <c r="G34">
+        <v>0.25</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35">
+        <v>62</v>
+      </c>
+      <c r="E35">
+        <v>0.2</v>
+      </c>
+      <c r="F35">
+        <v>0.35</v>
+      </c>
+      <c r="G35">
+        <v>0.5</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36">
+        <v>63</v>
+      </c>
+      <c r="E36">
+        <v>0.2</v>
+      </c>
+      <c r="F36">
+        <v>0.35</v>
+      </c>
+      <c r="G36">
+        <v>0.5</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37">
+        <v>64</v>
+      </c>
+      <c r="E37">
+        <v>0.2</v>
+      </c>
+      <c r="F37">
+        <v>0.35</v>
+      </c>
+      <c r="G37">
+        <v>0.5</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38">
         <v>65</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
         <v>1</v>
       </c>
     </row>
@@ -4934,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AE2EB2-CA42-4FE6-8F24-6446CEAEA505}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4953,7 +5053,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,7 +5074,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -5194,8 +5294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140C462A-14EE-4CAF-AB62-253A6557DD8D}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5210,7 +5310,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5231,7 +5331,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -5694,7 +5794,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:K19"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6162,8 +6262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D933BCA-4687-4E4C-BE87-A1256666CA3D}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6184,8 +6284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6284C5A4-23C7-4E9C-AAD3-20E9F77D80CA}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add AV2020 for P&F and Federeated
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_SJPF_Decrements_AV2019.xlsx
+++ b/inputs/data_raw/Data_SJPF_Decrements_AV2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_SJ\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C257B26A-0458-40EF-A43A-C5E955324648}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E0AE12-D7F0-4B88-B864-172988964762}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-26340" yWindow="5835" windowWidth="20910" windowHeight="13185" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="43" r:id="rId1"/>
@@ -384,7 +384,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -601,10 +601,10 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -710,24 +710,6 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="15"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -760,6 +742,24 @@
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="15"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1171,16 +1171,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>258046</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>353296</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>134160</xdr:rowOff>
+      <xdr:rowOff>77010</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1203,7 +1203,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1943100" y="1009650"/>
+          <a:off x="2647950" y="952500"/>
           <a:ext cx="6239746" cy="5801535"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1720,24 +1720,24 @@
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
     </row>
     <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="57" t="s">
         <v>55</v>
       </c>
       <c r="F7" t="s">
@@ -1788,19 +1788,19 @@
       <c r="C9">
         <v>55</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="58">
         <f>L$10/100</f>
         <v>0.02</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="58">
         <f t="shared" ref="E9:G9" si="0">M$10/100</f>
         <v>0.02</v>
       </c>
-      <c r="F9" s="64">
+      <c r="F9" s="58">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="G9" s="64">
+      <c r="G9" s="58">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
@@ -1813,19 +1813,19 @@
       <c r="C10">
         <v>56</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="58">
         <f>L$10/100</f>
         <v>0.02</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="58">
         <f t="shared" ref="E10" si="1">M$10/100</f>
         <v>0.02</v>
       </c>
-      <c r="F10" s="64">
+      <c r="F10" s="58">
         <f t="shared" ref="F10" si="2">N$10/100</f>
         <v>0.02</v>
       </c>
-      <c r="G10" s="64">
+      <c r="G10" s="58">
         <f t="shared" ref="G10" si="3">O$10/100</f>
         <v>0.05</v>
       </c>
@@ -1838,16 +1838,16 @@
       <c r="K10">
         <v>56</v>
       </c>
-      <c r="L10" s="64">
+      <c r="L10" s="58">
         <v>2</v>
       </c>
-      <c r="M10" s="64">
+      <c r="M10" s="58">
         <v>2</v>
       </c>
-      <c r="N10" s="64">
+      <c r="N10" s="58">
         <v>2</v>
       </c>
-      <c r="O10" s="65">
+      <c r="O10" s="59">
         <v>5</v>
       </c>
     </row>
@@ -2780,7 +2780,7 @@
         <v>35</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:E18" si="0">D8/100</f>
+        <f t="shared" ref="D18" si="0">D8/100</f>
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
@@ -2792,7 +2792,7 @@
         <v>40</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19:E19" si="1">D9/100</f>
+        <f t="shared" ref="D19" si="1">D9/100</f>
         <v>1.03E-2</v>
       </c>
     </row>
@@ -2804,7 +2804,7 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:E20" si="2">D10/100</f>
+        <f t="shared" ref="D20" si="2">D10/100</f>
         <v>1.32E-2</v>
       </c>
     </row>
@@ -2816,7 +2816,7 @@
         <v>50</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:E21" si="3">D11/100</f>
+        <f t="shared" ref="D21" si="3">D11/100</f>
         <v>2.7000000000000003E-2</v>
       </c>
     </row>
@@ -2828,7 +2828,7 @@
         <v>55</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:E22" si="4">D12/100</f>
+        <f t="shared" ref="D22" si="4">D12/100</f>
         <v>6.88E-2</v>
       </c>
     </row>
@@ -2840,7 +2840,7 @@
         <v>60</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:E23" si="5">D13/100</f>
+        <f t="shared" ref="D23" si="5">D13/100</f>
         <v>8.7100000000000011E-2</v>
       </c>
     </row>
@@ -2852,7 +2852,7 @@
         <v>65</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:E24" si="6">D14/100</f>
+        <f t="shared" ref="D24" si="6">D14/100</f>
         <v>0.1047</v>
       </c>
     </row>
@@ -2875,7 +2875,7 @@
         <v>30</v>
       </c>
       <c r="D26">
-        <f>E7/100</f>
+        <f t="shared" ref="D26:D33" si="7">E7/100</f>
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
         <v>35</v>
       </c>
       <c r="D27">
-        <f>E8/100</f>
+        <f t="shared" si="7"/>
         <v>1.5E-3</v>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
         <v>40</v>
       </c>
       <c r="D28">
-        <f>E9/100</f>
+        <f t="shared" si="7"/>
         <v>2.8000000000000004E-3</v>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
         <v>45</v>
       </c>
       <c r="D29">
-        <f>E10/100</f>
+        <f t="shared" si="7"/>
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -2923,7 +2923,7 @@
         <v>50</v>
       </c>
       <c r="D30">
-        <f>E11/100</f>
+        <f t="shared" si="7"/>
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
@@ -2935,7 +2935,7 @@
         <v>55</v>
       </c>
       <c r="D31">
-        <f>E12/100</f>
+        <f t="shared" si="7"/>
         <v>7.5399999999999995E-2</v>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
         <v>60</v>
       </c>
       <c r="D32">
-        <f>E13/100</f>
+        <f t="shared" si="7"/>
         <v>0.10769999999999999</v>
       </c>
     </row>
@@ -2959,7 +2959,7 @@
         <v>65</v>
       </c>
       <c r="D33">
-        <f>E14/100</f>
+        <f t="shared" si="7"/>
         <v>0.1484</v>
       </c>
     </row>
@@ -3716,30 +3716,30 @@
       <c r="C6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="61" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="68">
+      <c r="C8" s="62">
         <v>0</v>
       </c>
-      <c r="D8" s="69">
+      <c r="D8" s="63">
         <f>F8/100</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F8" s="66">
+      <c r="F8" s="60">
         <v>6.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="68">
-        <v>1</v>
-      </c>
-      <c r="D9" s="69">
+      <c r="C9" s="62">
+        <v>1</v>
+      </c>
+      <c r="D9" s="63">
         <f t="shared" ref="D9:D19" si="0">F9/100</f>
         <v>6.25E-2</v>
       </c>
@@ -3748,10 +3748,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="68">
+      <c r="C10" s="62">
         <v>2</v>
       </c>
-      <c r="D10" s="69">
+      <c r="D10" s="63">
         <f t="shared" si="0"/>
         <v>5.7500000000000002E-2</v>
       </c>
@@ -3760,10 +3760,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="68">
+      <c r="C11" s="62">
         <v>3</v>
       </c>
-      <c r="D11" s="69">
+      <c r="D11" s="63">
         <f t="shared" si="0"/>
         <v>5.2499999999999998E-2</v>
       </c>
@@ -3772,10 +3772,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="68">
+      <c r="C12" s="62">
         <v>4</v>
       </c>
-      <c r="D12" s="69">
+      <c r="D12" s="63">
         <f t="shared" si="0"/>
         <v>4.4999999999999998E-2</v>
       </c>
@@ -3784,10 +3784,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="68">
+      <c r="C13" s="62">
         <v>5</v>
       </c>
-      <c r="D13" s="69">
+      <c r="D13" s="63">
         <f t="shared" si="0"/>
         <v>3.7499999999999999E-2</v>
       </c>
@@ -3796,10 +3796,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="68">
+      <c r="C14" s="62">
         <v>6</v>
       </c>
-      <c r="D14" s="69">
+      <c r="D14" s="63">
         <f t="shared" si="0"/>
         <v>2.75E-2</v>
       </c>
@@ -3808,10 +3808,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="68">
+      <c r="C15" s="62">
         <v>7</v>
       </c>
-      <c r="D15" s="69">
+      <c r="D15" s="63">
         <f t="shared" si="0"/>
         <v>1.7500000000000002E-2</v>
       </c>
@@ -3820,10 +3820,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="68">
+      <c r="C16" s="62">
         <v>8</v>
       </c>
-      <c r="D16" s="69">
+      <c r="D16" s="63">
         <f t="shared" si="0"/>
         <v>1.2500000000000001E-2</v>
       </c>
@@ -3832,10 +3832,10 @@
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="68">
+      <c r="C17" s="62">
         <v>9</v>
       </c>
-      <c r="D17" s="69">
+      <c r="D17" s="63">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
@@ -3844,10 +3844,10 @@
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="68">
+      <c r="C18" s="62">
         <v>10</v>
       </c>
-      <c r="D18" s="69">
+      <c r="D18" s="63">
         <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
@@ -3856,10 +3856,10 @@
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="67">
+      <c r="C19" s="61">
         <v>11</v>
       </c>
-      <c r="D19" s="69">
+      <c r="D19" s="63">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3882,7 +3882,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5034,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AE2EB2-CA42-4FE6-8F24-6446CEAEA505}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5839,28 +5839,28 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54" t="s">
+      <c r="E6" s="66"/>
+      <c r="F6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54" t="s">
+      <c r="G6" s="67"/>
+      <c r="H6" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="54"/>
+      <c r="I6" s="67"/>
     </row>
     <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
@@ -6262,8 +6262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D933BCA-4687-4E4C-BE87-A1256666CA3D}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6318,13 +6318,13 @@
       <c r="C5" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="55" t="s">
         <v>53</v>
       </c>
       <c r="G5" s="25"/>
@@ -6333,10 +6333,10 @@
       <c r="J5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="57" t="s">
+      <c r="L5" s="51" t="s">
         <v>48</v>
       </c>
       <c r="M5" s="20" t="s">
@@ -6353,28 +6353,28 @@
       <c r="D6" s="23">
         <v>50</v>
       </c>
-      <c r="E6" s="60">
+      <c r="E6" s="54">
         <f>K6</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="F6" s="60">
-        <f t="shared" ref="F6:H6" si="0">L6</f>
+      <c r="F6" s="54">
+        <f t="shared" ref="F6" si="0">L6</f>
         <v>1</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="22">
         <v>50</v>
       </c>
-      <c r="K6" s="58">
+      <c r="K6" s="52">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L6" s="58">
-        <v>1</v>
-      </c>
-      <c r="M6" s="58">
+      <c r="L6" s="52">
+        <v>1</v>
+      </c>
+      <c r="M6" s="52">
         <v>0.35</v>
       </c>
-      <c r="N6" s="58">
+      <c r="N6" s="52">
         <v>1</v>
       </c>
     </row>
@@ -6385,28 +6385,28 @@
       <c r="D7" s="23">
         <v>51</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="54">
         <f>K7/100</f>
         <v>0.45</v>
       </c>
-      <c r="F7" s="60">
-        <f t="shared" ref="F7:H7" si="1">L7/100</f>
+      <c r="F7" s="54">
+        <f t="shared" ref="F7" si="1">L7/100</f>
         <v>1</v>
       </c>
       <c r="I7" s="26"/>
       <c r="J7" s="22">
         <v>51</v>
       </c>
-      <c r="K7" s="58">
+      <c r="K7" s="52">
         <v>45</v>
       </c>
-      <c r="L7" s="58">
+      <c r="L7" s="52">
         <v>100</v>
       </c>
-      <c r="M7" s="58">
+      <c r="M7" s="52">
         <v>35</v>
       </c>
-      <c r="N7" s="58">
+      <c r="N7" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6417,28 +6417,28 @@
       <c r="D8" s="23">
         <v>52</v>
       </c>
-      <c r="E8" s="60">
-        <f t="shared" ref="E8:E14" si="2">K8/100</f>
+      <c r="E8" s="54">
+        <f t="shared" ref="E8:E13" si="2">K8/100</f>
         <v>0.4</v>
       </c>
-      <c r="F8" s="60">
-        <f t="shared" ref="F8:F14" si="3">L8/100</f>
+      <c r="F8" s="54">
+        <f t="shared" ref="F8:F13" si="3">L8/100</f>
         <v>1</v>
       </c>
       <c r="I8" s="26"/>
       <c r="J8" s="22">
         <v>52</v>
       </c>
-      <c r="K8" s="58">
+      <c r="K8" s="52">
         <v>40</v>
       </c>
-      <c r="L8" s="58">
+      <c r="L8" s="52">
         <v>100</v>
       </c>
-      <c r="M8" s="58">
+      <c r="M8" s="52">
         <v>35</v>
       </c>
-      <c r="N8" s="58">
+      <c r="N8" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6449,11 +6449,11 @@
       <c r="D9" s="23">
         <v>53</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="54">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="F9" s="60">
+      <c r="F9" s="54">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6461,16 +6461,16 @@
       <c r="J9" s="22">
         <v>53</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K9" s="52">
         <v>30</v>
       </c>
-      <c r="L9" s="58">
+      <c r="L9" s="52">
         <v>100</v>
       </c>
-      <c r="M9" s="58">
+      <c r="M9" s="52">
         <v>35</v>
       </c>
-      <c r="N9" s="58">
+      <c r="N9" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6481,11 +6481,11 @@
       <c r="D10" s="23">
         <v>54</v>
       </c>
-      <c r="E10" s="60">
+      <c r="E10" s="54">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="F10" s="60">
+      <c r="F10" s="54">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6493,16 +6493,16 @@
       <c r="J10" s="22">
         <v>54</v>
       </c>
-      <c r="K10" s="58">
+      <c r="K10" s="52">
         <v>30</v>
       </c>
-      <c r="L10" s="58">
+      <c r="L10" s="52">
         <v>100</v>
       </c>
-      <c r="M10" s="58">
+      <c r="M10" s="52">
         <v>35</v>
       </c>
-      <c r="N10" s="58">
+      <c r="N10" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6513,11 +6513,11 @@
       <c r="D11" s="23">
         <v>55</v>
       </c>
-      <c r="E11" s="60">
+      <c r="E11" s="54">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="F11" s="60">
+      <c r="F11" s="54">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6525,16 +6525,16 @@
       <c r="J11" s="22">
         <v>55</v>
       </c>
-      <c r="K11" s="58">
+      <c r="K11" s="52">
         <v>30</v>
       </c>
-      <c r="L11" s="58">
+      <c r="L11" s="52">
         <v>100</v>
       </c>
-      <c r="M11" s="58">
+      <c r="M11" s="52">
         <v>30</v>
       </c>
-      <c r="N11" s="58">
+      <c r="N11" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6545,11 +6545,11 @@
       <c r="D12" s="23">
         <v>56</v>
       </c>
-      <c r="E12" s="60">
+      <c r="E12" s="54">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="F12" s="60">
+      <c r="F12" s="54">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6557,16 +6557,16 @@
       <c r="J12" s="22">
         <v>56</v>
       </c>
-      <c r="K12" s="58">
+      <c r="K12" s="52">
         <v>30</v>
       </c>
-      <c r="L12" s="58">
+      <c r="L12" s="52">
         <v>100</v>
       </c>
-      <c r="M12" s="58">
+      <c r="M12" s="52">
         <v>25</v>
       </c>
-      <c r="N12" s="58">
+      <c r="N12" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6577,11 +6577,11 @@
       <c r="D13" s="23">
         <v>57</v>
       </c>
-      <c r="E13" s="60">
+      <c r="E13" s="54">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="F13" s="60">
+      <c r="F13" s="54">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -6589,16 +6589,16 @@
       <c r="J13" s="22">
         <v>57</v>
       </c>
-      <c r="K13" s="58">
+      <c r="K13" s="52">
         <v>30</v>
       </c>
-      <c r="L13" s="58">
+      <c r="L13" s="52">
         <v>100</v>
       </c>
-      <c r="M13" s="58">
+      <c r="M13" s="52">
         <v>20</v>
       </c>
-      <c r="N13" s="58">
+      <c r="N13" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6609,12 +6609,12 @@
       <c r="D14" s="23">
         <v>58</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="54">
         <f>K$14/100</f>
         <v>0.5</v>
       </c>
-      <c r="F14" s="60">
-        <f t="shared" ref="F14:H17" si="4">L$14/100</f>
+      <c r="F14" s="54">
+        <f t="shared" ref="F14:F17" si="4">L$14/100</f>
         <v>1</v>
       </c>
       <c r="I14" s="23">
@@ -6623,16 +6623,16 @@
       <c r="J14" s="22">
         <v>-61</v>
       </c>
-      <c r="K14" s="58">
-        <v>50</v>
-      </c>
-      <c r="L14" s="58">
+      <c r="K14" s="52">
+        <v>50</v>
+      </c>
+      <c r="L14" s="52">
         <v>100</v>
       </c>
-      <c r="M14" s="58">
+      <c r="M14" s="52">
         <v>27.5</v>
       </c>
-      <c r="N14" s="58">
+      <c r="N14" s="52">
         <v>100</v>
       </c>
     </row>
@@ -6643,11 +6643,11 @@
       <c r="D15" s="23">
         <v>59</v>
       </c>
-      <c r="E15" s="60">
+      <c r="E15" s="54">
         <f>K$14/100</f>
         <v>0.5</v>
       </c>
-      <c r="F15" s="60">
+      <c r="F15" s="54">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -6655,16 +6655,16 @@
       <c r="J15" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K15" s="53">
         <v>100</v>
       </c>
-      <c r="L15" s="59">
+      <c r="L15" s="53">
         <v>100</v>
       </c>
-      <c r="M15" s="59">
+      <c r="M15" s="53">
         <v>100</v>
       </c>
-      <c r="N15" s="59">
+      <c r="N15" s="53">
         <v>100</v>
       </c>
     </row>
@@ -6675,11 +6675,11 @@
       <c r="D16" s="23">
         <v>60</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="54">
         <f>K$14/100</f>
         <v>0.5</v>
       </c>
-      <c r="F16" s="60">
+      <c r="F16" s="54">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -6691,11 +6691,11 @@
       <c r="D17" s="23">
         <v>61</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="54">
         <f>K$14/100</f>
         <v>0.5</v>
       </c>
-      <c r="F17" s="60">
+      <c r="F17" s="54">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -6707,12 +6707,12 @@
       <c r="D18" s="23">
         <v>62</v>
       </c>
-      <c r="E18" s="60">
+      <c r="E18" s="54">
         <f>K15/100</f>
         <v>1</v>
       </c>
-      <c r="F18" s="60">
-        <f t="shared" ref="F18:H18" si="5">L15/100</f>
+      <c r="F18" s="54">
+        <f t="shared" ref="F18" si="5">L15/100</f>
         <v>1</v>
       </c>
     </row>
@@ -6723,11 +6723,11 @@
       <c r="D19" s="23">
         <v>50</v>
       </c>
-      <c r="E19" s="60">
+      <c r="E19" s="54">
         <f>M6</f>
         <v>0.35</v>
       </c>
-      <c r="F19" s="60">
+      <c r="F19" s="54">
         <f>N6</f>
         <v>1</v>
       </c>
@@ -6739,12 +6739,12 @@
       <c r="D20" s="23">
         <v>51</v>
       </c>
-      <c r="E20" s="60">
-        <f>M7/100</f>
+      <c r="E20" s="54">
+        <f t="shared" ref="E20:F26" si="6">M7/100</f>
         <v>0.35</v>
       </c>
-      <c r="F20" s="60">
-        <f>N7/100</f>
+      <c r="F20" s="54">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6755,12 +6755,12 @@
       <c r="D21" s="23">
         <v>52</v>
       </c>
-      <c r="E21" s="60">
-        <f>M8/100</f>
+      <c r="E21" s="54">
+        <f t="shared" si="6"/>
         <v>0.35</v>
       </c>
-      <c r="F21" s="60">
-        <f>N8/100</f>
+      <c r="F21" s="54">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6771,12 +6771,12 @@
       <c r="D22" s="23">
         <v>53</v>
       </c>
-      <c r="E22" s="60">
-        <f>M9/100</f>
+      <c r="E22" s="54">
+        <f t="shared" si="6"/>
         <v>0.35</v>
       </c>
-      <c r="F22" s="60">
-        <f>N9/100</f>
+      <c r="F22" s="54">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6787,12 +6787,12 @@
       <c r="D23" s="23">
         <v>54</v>
       </c>
-      <c r="E23" s="60">
-        <f>M10/100</f>
+      <c r="E23" s="54">
+        <f t="shared" si="6"/>
         <v>0.35</v>
       </c>
-      <c r="F23" s="60">
-        <f>N10/100</f>
+      <c r="F23" s="54">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6803,12 +6803,12 @@
       <c r="D24" s="23">
         <v>55</v>
       </c>
-      <c r="E24" s="60">
-        <f>M11/100</f>
+      <c r="E24" s="54">
+        <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="F24" s="60">
-        <f>N11/100</f>
+      <c r="F24" s="54">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6819,12 +6819,12 @@
       <c r="D25" s="23">
         <v>56</v>
       </c>
-      <c r="E25" s="60">
-        <f>M12/100</f>
+      <c r="E25" s="54">
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
-      <c r="F25" s="60">
-        <f>N12/100</f>
+      <c r="F25" s="54">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6835,12 +6835,12 @@
       <c r="D26" s="23">
         <v>57</v>
       </c>
-      <c r="E26" s="60">
-        <f>M13/100</f>
+      <c r="E26" s="54">
+        <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
-      <c r="F26" s="60">
-        <f>N13/100</f>
+      <c r="F26" s="54">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6851,12 +6851,12 @@
       <c r="D27" s="23">
         <v>58</v>
       </c>
-      <c r="E27" s="60">
-        <f>M$14/100</f>
+      <c r="E27" s="54">
+        <f t="shared" ref="E27:F30" si="7">M$14/100</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="F27" s="60">
-        <f>N$14/100</f>
+      <c r="F27" s="54">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6867,12 +6867,12 @@
       <c r="D28" s="23">
         <v>59</v>
       </c>
-      <c r="E28" s="60">
-        <f>M$14/100</f>
+      <c r="E28" s="54">
+        <f t="shared" si="7"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="F28" s="60">
-        <f>N$14/100</f>
+      <c r="F28" s="54">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6883,12 +6883,12 @@
       <c r="D29" s="23">
         <v>60</v>
       </c>
-      <c r="E29" s="60">
-        <f>M$14/100</f>
+      <c r="E29" s="54">
+        <f t="shared" si="7"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="F29" s="60">
-        <f>N$14/100</f>
+      <c r="F29" s="54">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6899,12 +6899,12 @@
       <c r="D30" s="23">
         <v>61</v>
       </c>
-      <c r="E30" s="60">
-        <f>M$14/100</f>
+      <c r="E30" s="54">
+        <f t="shared" si="7"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="F30" s="60">
-        <f>N$14/100</f>
+      <c r="F30" s="54">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6915,11 +6915,11 @@
       <c r="D31" s="23">
         <v>62</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="54">
         <f>M15/100</f>
         <v>1</v>
       </c>
-      <c r="F31" s="60">
+      <c r="F31" s="54">
         <f>N15/100</f>
         <v>1</v>
       </c>

</xml_diff>